<commit_message>
More parm sweep scenarios.
</commit_message>
<xml_diff>
--- a/SimplePowerSector.xlsx
+++ b/SimplePowerSector.xlsx
@@ -200,9 +200,6 @@
     <t>Mfg.n</t>
   </si>
   <si>
-    <t xml:space="preserve">2. ysum = TFO*f </t>
-  </si>
-  <si>
     <t xml:space="preserve">7. V = D*q_hat </t>
   </si>
   <si>
@@ -336,6 +333,9 @@
   </si>
   <si>
     <t>5c. A = Z * D</t>
+  </si>
+  <si>
+    <t>2. ysum = TFO*f.split</t>
   </si>
 </sst>
 </file>
@@ -802,24 +802,58 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -829,45 +863,11 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1043,6 +1043,54 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="4" name="AutoShape 2"/>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9934575" cy="9572625"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst/>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:round/>
+          <a:headEnd/>
+          <a:tailEnd/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="AutoShape 2"/>
         <xdr:cNvSpPr>
           <a:spLocks noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -1343,8 +1391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BO1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="M48" sqref="M48"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="AC13" sqref="AC13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1416,14 +1464,14 @@
       <c r="BC1" s="5"/>
       <c r="BD1" s="5"/>
       <c r="BE1" s="6"/>
-      <c r="BF1" s="89" t="s">
+      <c r="BF1" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="BG1" s="76"/>
-      <c r="BH1" s="76"/>
-      <c r="BI1" s="76"/>
-      <c r="BJ1" s="76"/>
-      <c r="BK1" s="76"/>
+      <c r="BG1" s="77"/>
+      <c r="BH1" s="77"/>
+      <c r="BI1" s="77"/>
+      <c r="BJ1" s="77"/>
+      <c r="BK1" s="77"/>
       <c r="BL1" s="7"/>
       <c r="BM1" s="7"/>
       <c r="BN1" s="7"/>
@@ -1431,43 +1479,43 @@
     </row>
     <row r="2" spans="1:67" x14ac:dyDescent="0.2">
       <c r="C2" s="4"/>
-      <c r="D2" s="78" t="s">
+      <c r="D2" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="77"/>
+      <c r="G2" s="77"/>
       <c r="H2" s="8"/>
       <c r="I2" s="2"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="80" t="s">
+      <c r="M2" s="83" t="s">
         <v>5</v>
       </c>
-      <c r="N2" s="76"/>
+      <c r="N2" s="77"/>
       <c r="O2" s="9"/>
       <c r="P2" s="9"/>
       <c r="Q2" s="9"/>
       <c r="R2" s="9"/>
       <c r="S2" s="10"/>
-      <c r="T2" s="94" t="s">
+      <c r="T2" s="87" t="s">
         <v>6</v>
       </c>
-      <c r="U2" s="76"/>
-      <c r="V2" s="76"/>
-      <c r="W2" s="76"/>
-      <c r="X2" s="76"/>
+      <c r="U2" s="77"/>
+      <c r="V2" s="77"/>
+      <c r="W2" s="77"/>
+      <c r="X2" s="77"/>
       <c r="Y2" s="11"/>
-      <c r="Z2" s="85" t="s">
+      <c r="Z2" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="76"/>
-      <c r="AB2" s="76"/>
-      <c r="AC2" s="86" t="s">
+      <c r="AA2" s="77"/>
+      <c r="AB2" s="77"/>
+      <c r="AC2" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="76"/>
+      <c r="AD2" s="77"/>
       <c r="AG2" s="12"/>
       <c r="AH2" s="12" t="s">
         <v>9</v>
@@ -1480,12 +1528,12 @@
       <c r="BC2" s="5"/>
       <c r="BD2" s="5"/>
       <c r="BE2" s="6"/>
-      <c r="BF2" s="76"/>
-      <c r="BG2" s="76"/>
-      <c r="BH2" s="76"/>
-      <c r="BI2" s="76"/>
-      <c r="BJ2" s="76"/>
-      <c r="BK2" s="76"/>
+      <c r="BF2" s="77"/>
+      <c r="BG2" s="77"/>
+      <c r="BH2" s="77"/>
+      <c r="BI2" s="77"/>
+      <c r="BJ2" s="77"/>
+      <c r="BK2" s="77"/>
       <c r="BL2" s="7"/>
       <c r="BM2" s="7"/>
       <c r="BN2" s="7"/>
@@ -1497,10 +1545,10 @@
       <c r="E3" s="15">
         <v>200</v>
       </c>
-      <c r="F3" s="79" t="s">
+      <c r="F3" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="76"/>
+      <c r="G3" s="77"/>
       <c r="H3" s="16"/>
       <c r="I3" s="17"/>
       <c r="J3" s="3"/>
@@ -1588,12 +1636,12 @@
       <c r="BC3" s="5"/>
       <c r="BD3" s="5"/>
       <c r="BE3" s="6"/>
-      <c r="BF3" s="76"/>
-      <c r="BG3" s="76"/>
-      <c r="BH3" s="76"/>
-      <c r="BI3" s="76"/>
-      <c r="BJ3" s="76"/>
-      <c r="BK3" s="76"/>
+      <c r="BF3" s="77"/>
+      <c r="BG3" s="77"/>
+      <c r="BH3" s="77"/>
+      <c r="BI3" s="77"/>
+      <c r="BJ3" s="77"/>
+      <c r="BK3" s="77"/>
       <c r="BL3" s="7"/>
       <c r="BM3" s="7"/>
       <c r="BN3" s="7"/>
@@ -1612,38 +1660,38 @@
       <c r="Q4" s="18"/>
       <c r="R4" s="18"/>
       <c r="S4" s="4"/>
-      <c r="T4" s="83" t="s">
-        <v>89</v>
-      </c>
-      <c r="U4" s="76"/>
-      <c r="V4" s="76"/>
-      <c r="W4" s="76"/>
-      <c r="X4" s="76"/>
-      <c r="Y4" s="76"/>
+      <c r="T4" s="97" t="s">
+        <v>88</v>
+      </c>
+      <c r="U4" s="77"/>
+      <c r="V4" s="77"/>
+      <c r="W4" s="77"/>
+      <c r="X4" s="77"/>
+      <c r="Y4" s="77"/>
       <c r="Z4" s="19"/>
       <c r="AA4" s="19"/>
       <c r="AB4" s="19"/>
-      <c r="AC4" s="81" t="s">
+      <c r="AC4" s="95" t="s">
         <v>26</v>
       </c>
-      <c r="AD4" s="82"/>
+      <c r="AD4" s="96"/>
       <c r="AE4" s="18"/>
       <c r="AF4" s="22" t="s">
         <v>27</v>
       </c>
       <c r="AG4" s="21"/>
-      <c r="AH4" s="99" t="s">
-        <v>93</v>
+      <c r="AH4" s="75" t="s">
+        <v>92</v>
       </c>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="45"/>
       <c r="AK4" s="45"/>
-      <c r="AL4" s="74" t="s">
-        <v>86</v>
-      </c>
-      <c r="AM4" s="74"/>
-      <c r="AN4" s="74"/>
-      <c r="AO4" s="74"/>
+      <c r="AL4" s="98" t="s">
+        <v>85</v>
+      </c>
+      <c r="AM4" s="98"/>
+      <c r="AN4" s="98"/>
+      <c r="AO4" s="98"/>
       <c r="AQ4" s="2"/>
       <c r="AR4" s="13"/>
       <c r="AS4" s="18" t="s">
@@ -1686,13 +1734,13 @@
     </row>
     <row r="5" spans="1:67" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="C5" s="4"/>
-      <c r="D5" s="80" t="s">
+      <c r="D5" s="83" t="s">
         <v>29</v>
       </c>
-      <c r="E5" s="76"/>
+      <c r="E5" s="77"/>
       <c r="I5" s="2"/>
       <c r="J5" s="27"/>
-      <c r="K5" s="75" t="s">
+      <c r="K5" s="76" t="s">
         <v>5</v>
       </c>
       <c r="L5" s="18" t="s">
@@ -1808,11 +1856,11 @@
       </c>
       <c r="BE5" s="2"/>
       <c r="BF5" s="31"/>
-      <c r="BG5" s="90" t="s">
+      <c r="BG5" s="79" t="s">
         <v>30</v>
       </c>
-      <c r="BH5" s="91"/>
-      <c r="BI5" s="91"/>
+      <c r="BH5" s="80"/>
+      <c r="BI5" s="80"/>
       <c r="BJ5" s="32" t="s">
         <v>31</v>
       </c>
@@ -1823,13 +1871,13 @@
     </row>
     <row r="6" spans="1:67" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C6" s="4"/>
-      <c r="D6" s="79" t="s">
+      <c r="D6" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="76"/>
+      <c r="E6" s="77"/>
       <c r="I6" s="2"/>
       <c r="J6" s="27"/>
-      <c r="K6" s="76"/>
+      <c r="K6" s="77"/>
       <c r="L6" s="18" t="s">
         <v>13</v>
       </c>
@@ -1944,9 +1992,9 @@
       <c r="BF6" s="33" t="s">
         <v>33</v>
       </c>
-      <c r="BG6" s="92"/>
-      <c r="BH6" s="92"/>
-      <c r="BI6" s="92"/>
+      <c r="BG6" s="81"/>
+      <c r="BH6" s="81"/>
+      <c r="BI6" s="81"/>
       <c r="BJ6" s="33" t="s">
         <v>34</v>
       </c>
@@ -1972,7 +2020,7 @@
       <c r="F7" s="9"/>
       <c r="I7" s="2"/>
       <c r="J7" s="27"/>
-      <c r="K7" s="76"/>
+      <c r="K7" s="77"/>
       <c r="L7" s="18" t="s">
         <v>14</v>
       </c>
@@ -2104,14 +2152,14 @@
       <c r="E8" s="37">
         <v>0.4</v>
       </c>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="G8" s="76"/>
+      <c r="G8" s="77"/>
       <c r="H8" s="16"/>
       <c r="I8" s="38"/>
       <c r="J8" s="27"/>
-      <c r="K8" s="76"/>
+      <c r="K8" s="77"/>
       <c r="L8" s="18" t="s">
         <v>15</v>
       </c>
@@ -2236,7 +2284,7 @@
     <row r="9" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I9" s="38"/>
       <c r="J9" s="27"/>
-      <c r="K9" s="76"/>
+      <c r="K9" s="77"/>
       <c r="L9" s="18" t="s">
         <v>16</v>
       </c>
@@ -2349,10 +2397,10 @@
       <c r="BE9" s="2"/>
     </row>
     <row r="10" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B10" s="75" t="s">
+      <c r="B10" s="76" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="87" t="s">
+      <c r="C10" s="90" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="39">
@@ -2361,10 +2409,10 @@
       <c r="E10" s="39">
         <v>0</v>
       </c>
-      <c r="F10" s="84" t="s">
+      <c r="F10" s="85" t="s">
         <v>46</v>
       </c>
-      <c r="G10" s="76"/>
+      <c r="G10" s="77"/>
       <c r="H10" s="8"/>
       <c r="I10" s="38"/>
       <c r="L10" s="18" t="s">
@@ -2456,16 +2504,16 @@
     </row>
     <row r="11" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="13"/>
-      <c r="B11" s="76"/>
-      <c r="C11" s="76"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="77"/>
       <c r="D11" s="39">
         <v>0</v>
       </c>
       <c r="E11" s="39">
         <v>0</v>
       </c>
-      <c r="F11" s="76"/>
-      <c r="G11" s="76"/>
+      <c r="F11" s="77"/>
+      <c r="G11" s="77"/>
       <c r="H11" s="8"/>
       <c r="I11" s="38"/>
       <c r="L11" s="40"/>
@@ -2536,7 +2584,7 @@
     </row>
     <row r="12" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="13"/>
-      <c r="B12" s="76"/>
+      <c r="B12" s="77"/>
       <c r="C12" s="88" t="s">
         <v>50</v>
       </c>
@@ -2546,8 +2594,8 @@
       <c r="E12" s="39">
         <v>0.4</v>
       </c>
-      <c r="F12" s="76"/>
-      <c r="G12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="77"/>
       <c r="H12" s="8"/>
       <c r="I12" s="38"/>
       <c r="L12" s="21"/>
@@ -2559,7 +2607,7 @@
       <c r="R12" s="4"/>
       <c r="Z12" s="4"/>
       <c r="AC12" s="23" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="AH12" s="4"/>
       <c r="AI12" s="45"/>
@@ -2596,16 +2644,16 @@
       <c r="BE12" s="2"/>
     </row>
     <row r="13" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B13" s="76"/>
-      <c r="C13" s="76"/>
+      <c r="B13" s="77"/>
+      <c r="C13" s="77"/>
       <c r="D13" s="39">
         <v>0.25</v>
       </c>
       <c r="E13" s="39">
         <v>0.2</v>
       </c>
-      <c r="F13" s="76"/>
-      <c r="G13" s="76"/>
+      <c r="F13" s="77"/>
+      <c r="G13" s="77"/>
       <c r="H13" s="8"/>
       <c r="I13" s="2"/>
       <c r="M13" s="46"/>
@@ -2651,26 +2699,26 @@
     </row>
     <row r="14" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="13"/>
-      <c r="B14" s="76"/>
-      <c r="C14" s="76"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="77"/>
       <c r="D14" s="39">
         <v>0.4</v>
       </c>
       <c r="E14" s="39">
         <v>0.3</v>
       </c>
-      <c r="F14" s="76"/>
-      <c r="G14" s="76"/>
+      <c r="F14" s="77"/>
+      <c r="G14" s="77"/>
       <c r="H14" s="8"/>
       <c r="I14" s="2"/>
-      <c r="M14" s="95" t="s">
-        <v>52</v>
-      </c>
-      <c r="N14" s="76"/>
-      <c r="O14" s="76"/>
-      <c r="P14" s="76"/>
-      <c r="Q14" s="76"/>
-      <c r="R14" s="76"/>
+      <c r="M14" s="89" t="s">
+        <v>51</v>
+      </c>
+      <c r="N14" s="77"/>
+      <c r="O14" s="77"/>
+      <c r="P14" s="77"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="77"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -2681,17 +2729,17 @@
       <c r="Z14" s="4"/>
       <c r="AG14" s="21"/>
       <c r="AH14" s="73" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="AI14" s="4"/>
-      <c r="AJ14" s="74" t="s">
-        <v>90</v>
-      </c>
-      <c r="AK14" s="74"/>
-      <c r="AL14" s="74"/>
-      <c r="AM14" s="74"/>
-      <c r="AN14" s="74"/>
-      <c r="AO14" s="74"/>
+      <c r="AJ14" s="98" t="s">
+        <v>89</v>
+      </c>
+      <c r="AK14" s="98"/>
+      <c r="AL14" s="98"/>
+      <c r="AM14" s="98"/>
+      <c r="AN14" s="98"/>
+      <c r="AO14" s="98"/>
       <c r="AQ14" s="2"/>
       <c r="AS14" s="18" t="s">
         <v>20</v>
@@ -2719,19 +2767,19 @@
       <c r="BE14" s="2"/>
     </row>
     <row r="15" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
+      <c r="B15" s="77"/>
+      <c r="C15" s="77"/>
       <c r="D15" s="39">
         <v>0.1</v>
       </c>
       <c r="E15" s="39">
         <v>0.1</v>
       </c>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="77"/>
       <c r="I15" s="2"/>
       <c r="J15" s="27"/>
-      <c r="K15" s="75" t="s">
+      <c r="K15" s="76" t="s">
         <v>6</v>
       </c>
       <c r="L15" s="18" t="s">
@@ -2824,7 +2872,7 @@
     <row r="16" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="I16" s="2"/>
       <c r="J16" s="27"/>
-      <c r="K16" s="76"/>
+      <c r="K16" s="77"/>
       <c r="L16" s="18" t="s">
         <v>19</v>
       </c>
@@ -2914,14 +2962,14 @@
     </row>
     <row r="17" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="C17" s="51" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="27"/>
-      <c r="K17" s="76"/>
+      <c r="K17" s="77"/>
       <c r="L17" s="18" t="s">
         <v>20</v>
       </c>
@@ -2998,21 +3046,21 @@
       <c r="BO17" s="18"/>
     </row>
     <row r="18" spans="1:67" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="84" t="s">
-        <v>91</v>
-      </c>
-      <c r="B18" s="76"/>
-      <c r="C18" s="80" t="s">
+      <c r="A18" s="85" t="s">
+        <v>90</v>
+      </c>
+      <c r="B18" s="77"/>
+      <c r="C18" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
+      <c r="D18" s="77"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="77"/>
+      <c r="G18" s="77"/>
+      <c r="H18" s="77"/>
       <c r="I18" s="38"/>
       <c r="J18" s="27"/>
-      <c r="K18" s="76"/>
+      <c r="K18" s="77"/>
       <c r="L18" s="18" t="s">
         <v>21</v>
       </c>
@@ -3092,21 +3140,21 @@
       <c r="BO18" s="18"/>
     </row>
     <row r="19" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="79" t="s">
+      <c r="A19" s="77"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="76"/>
-      <c r="E19" s="79" t="s">
+      <c r="D19" s="77"/>
+      <c r="E19" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
+      <c r="F19" s="77"/>
+      <c r="G19" s="77"/>
+      <c r="H19" s="77"/>
       <c r="I19" s="38"/>
       <c r="J19" s="27"/>
-      <c r="K19" s="76"/>
+      <c r="K19" s="77"/>
       <c r="L19" s="18" t="s">
         <v>22</v>
       </c>
@@ -3190,8 +3238,8 @@
       <c r="BO19" s="18"/>
     </row>
     <row r="20" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
+      <c r="A20" s="77"/>
+      <c r="B20" s="77"/>
       <c r="C20" s="9" t="s">
         <v>18</v>
       </c>
@@ -3295,10 +3343,10 @@
       <c r="BO20" s="18"/>
     </row>
     <row r="21" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B21" s="87" t="s">
+      <c r="B21" s="90" t="s">
         <v>45</v>
       </c>
       <c r="C21" s="39">
@@ -3327,7 +3375,7 @@
       <c r="AD21" s="56"/>
       <c r="AE21" s="57"/>
       <c r="AF21" s="57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AH21" s="47">
         <f ca="1">SUM(AH15:AH19)</f>
@@ -3343,8 +3391,8 @@
       <c r="BO21" s="18"/>
     </row>
     <row r="22" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="76"/>
-      <c r="B22" s="76"/>
+      <c r="A22" s="77"/>
+      <c r="B22" s="77"/>
       <c r="C22" s="39">
         <v>0</v>
       </c>
@@ -3365,7 +3413,7 @@
       </c>
       <c r="I22" s="38"/>
       <c r="L22" s="58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M22" s="30">
         <f t="array" ref="M22:R22">TRANSPOSE(AH5:AH10)</f>
@@ -3387,7 +3435,7 @@
         <v>20</v>
       </c>
       <c r="S22" s="59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="T22" s="60">
         <f t="array" aca="1" ref="T22:Y22" ca="1">TRANSPOSE(AH15:AH20)</f>
@@ -3420,7 +3468,7 @@
       <c r="BE22" s="2"/>
     </row>
     <row r="23" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A23" s="76"/>
+      <c r="A23" s="77"/>
       <c r="B23" s="88" t="s">
         <v>50</v>
       </c>
@@ -3453,7 +3501,7 @@
       <c r="AD23" s="4"/>
       <c r="AE23" s="12"/>
       <c r="AF23" s="58" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG23" s="21"/>
       <c r="AH23" s="61">
@@ -3464,8 +3512,8 @@
       <c r="BE23" s="2"/>
     </row>
     <row r="24" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A24" s="76"/>
-      <c r="B24" s="76"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="77"/>
       <c r="C24" s="39">
         <v>0</v>
       </c>
@@ -3486,7 +3534,7 @@
       </c>
       <c r="I24" s="2"/>
       <c r="L24" s="14" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA24" s="47"/>
       <c r="AG24" s="4"/>
@@ -3495,8 +3543,8 @@
       <c r="BE24" s="2"/>
     </row>
     <row r="25" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A25" s="76"/>
-      <c r="B25" s="76"/>
+      <c r="A25" s="77"/>
+      <c r="B25" s="77"/>
       <c r="C25" s="39">
         <v>0</v>
       </c>
@@ -3520,7 +3568,7 @@
         <v>12</v>
       </c>
       <c r="M25" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA25" s="4"/>
       <c r="AB25" s="4"/>
@@ -3534,8 +3582,8 @@
       <c r="BE25" s="2"/>
     </row>
     <row r="26" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="76"/>
-      <c r="B26" s="76"/>
+      <c r="A26" s="77"/>
+      <c r="B26" s="77"/>
       <c r="C26" s="39">
         <v>0</v>
       </c>
@@ -3559,7 +3607,7 @@
         <v>13</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA26" s="13"/>
       <c r="AB26" s="13"/>
@@ -3585,7 +3633,7 @@
         <v>14</v>
       </c>
       <c r="M27" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="U27" s="70">
         <f ca="1">IF((ROW()-ROW($BQ$26))=(COLUMN()-COLUMN($BQ$26)),INDIRECT("BC"&amp;ROW()),0)</f>
@@ -3601,7 +3649,7 @@
     </row>
     <row r="28" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B28" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="64">
         <v>1</v>
@@ -3626,7 +3674,7 @@
         <v>15</v>
       </c>
       <c r="M28" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AA28" s="13"/>
       <c r="AB28" s="13"/>
@@ -3640,22 +3688,22 @@
       <c r="BE28" s="2"/>
     </row>
     <row r="29" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A29" s="93" t="s">
-        <v>92</v>
-      </c>
-      <c r="B29" s="76"/>
-      <c r="C29" s="76"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="76"/>
-      <c r="G29" s="76"/>
-      <c r="H29" s="76"/>
+      <c r="A29" s="84" t="s">
+        <v>91</v>
+      </c>
+      <c r="B29" s="77"/>
+      <c r="C29" s="77"/>
+      <c r="D29" s="77"/>
+      <c r="E29" s="77"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
       <c r="I29" s="2"/>
       <c r="L29" s="18" t="s">
         <v>16</v>
       </c>
       <c r="M29" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AG29" s="4"/>
       <c r="AH29" s="4"/>
@@ -3663,24 +3711,24 @@
       <c r="BE29" s="2"/>
     </row>
     <row r="30" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A30" s="96" t="s">
-        <v>94</v>
-      </c>
-      <c r="B30" s="97"/>
-      <c r="C30" s="80" t="s">
+      <c r="A30" s="93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30" s="94"/>
+      <c r="C30" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="D30" s="76"/>
-      <c r="E30" s="76"/>
-      <c r="F30" s="76"/>
-      <c r="G30" s="76"/>
-      <c r="H30" s="76"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
       <c r="I30" s="2"/>
       <c r="L30" s="18" t="s">
         <v>17</v>
       </c>
       <c r="M30" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AG30" s="4"/>
       <c r="AH30" s="4"/>
@@ -3688,18 +3736,18 @@
       <c r="BE30" s="2"/>
     </row>
     <row r="31" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A31" s="97"/>
-      <c r="B31" s="97"/>
-      <c r="C31" s="79" t="s">
+      <c r="A31" s="94"/>
+      <c r="B31" s="94"/>
+      <c r="C31" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="79" t="s">
+      <c r="D31" s="77"/>
+      <c r="E31" s="82" t="s">
         <v>50</v>
       </c>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
-      <c r="H31" s="76"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
       <c r="I31" s="2"/>
       <c r="L31" s="21"/>
       <c r="AG31" s="4"/>
@@ -3708,8 +3756,8 @@
       <c r="BE31" s="2"/>
     </row>
     <row r="32" spans="1:67" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="97"/>
-      <c r="B32" s="97"/>
+      <c r="A32" s="94"/>
+      <c r="B32" s="94"/>
       <c r="C32" s="9" t="s">
         <v>18</v>
       </c>
@@ -3733,7 +3781,7 @@
         <v>18</v>
       </c>
       <c r="M32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AG32" s="4"/>
       <c r="AH32" s="4"/>
@@ -3741,10 +3789,10 @@
       <c r="BE32" s="2"/>
     </row>
     <row r="33" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="B33" s="87" t="s">
+      <c r="B33" s="90" t="s">
         <v>45</v>
       </c>
       <c r="C33" s="39">
@@ -3774,7 +3822,7 @@
         <v>19</v>
       </c>
       <c r="M33" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AG33" s="4"/>
       <c r="AH33" s="4"/>
@@ -3782,8 +3830,8 @@
       <c r="BE33" s="2"/>
     </row>
     <row r="34" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A34" s="76"/>
-      <c r="B34" s="76"/>
+      <c r="A34" s="77"/>
+      <c r="B34" s="77"/>
       <c r="C34" s="39">
         <v>0</v>
       </c>
@@ -3811,7 +3859,7 @@
         <v>20</v>
       </c>
       <c r="M34" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AG34" s="4"/>
       <c r="AH34" s="4"/>
@@ -3819,7 +3867,7 @@
       <c r="BE34" s="2"/>
     </row>
     <row r="35" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A35" s="76"/>
+      <c r="A35" s="77"/>
       <c r="B35" s="88" t="s">
         <v>50</v>
       </c>
@@ -3850,7 +3898,7 @@
         <v>21</v>
       </c>
       <c r="M35" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AG35" s="4"/>
       <c r="AH35" s="4"/>
@@ -3858,8 +3906,8 @@
       <c r="BE35" s="2"/>
     </row>
     <row r="36" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="76"/>
-      <c r="B36" s="76"/>
+      <c r="A36" s="77"/>
+      <c r="B36" s="77"/>
       <c r="C36" s="39">
         <v>0</v>
       </c>
@@ -3887,7 +3935,7 @@
         <v>22</v>
       </c>
       <c r="M36" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="U36" s="3"/>
       <c r="AG36" s="4"/>
@@ -3896,8 +3944,8 @@
       <c r="BE36" s="2"/>
     </row>
     <row r="37" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A37" s="76"/>
-      <c r="B37" s="76"/>
+      <c r="A37" s="77"/>
+      <c r="B37" s="77"/>
       <c r="C37" s="39">
         <v>0</v>
       </c>
@@ -3925,7 +3973,7 @@
         <v>23</v>
       </c>
       <c r="M37" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AG37" s="4"/>
       <c r="AH37" s="4"/>
@@ -3933,8 +3981,8 @@
       <c r="BE37" s="2"/>
     </row>
     <row r="38" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A38" s="76"/>
-      <c r="B38" s="76"/>
+      <c r="A38" s="77"/>
+      <c r="B38" s="77"/>
       <c r="C38" s="39">
         <v>0</v>
       </c>
@@ -3972,7 +4020,7 @@
         <v>24</v>
       </c>
       <c r="M39" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q39" s="3"/>
       <c r="R39" s="3"/>
@@ -3987,7 +4035,7 @@
         <v>25</v>
       </c>
       <c r="M40" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="AG40" s="4"/>
       <c r="AH40" s="4"/>
@@ -3996,7 +4044,7 @@
     </row>
     <row r="41" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A41" s="72" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G41" s="3"/>
       <c r="I41" s="2"/>
@@ -4006,14 +4054,14 @@
       <c r="BE41" s="2"/>
     </row>
     <row r="42" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="C42" s="77" t="s">
+      <c r="C42" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="77"/>
-      <c r="E42" s="77"/>
-      <c r="F42" s="77"/>
-      <c r="G42" s="77"/>
-      <c r="H42" s="77"/>
+      <c r="D42" s="99"/>
+      <c r="E42" s="99"/>
+      <c r="F42" s="99"/>
+      <c r="G42" s="99"/>
+      <c r="H42" s="99"/>
       <c r="I42" s="66"/>
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
@@ -4030,10 +4078,10 @@
       <c r="BE42" s="2"/>
     </row>
     <row r="43" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A43" s="98" t="s">
-        <v>95</v>
-      </c>
-      <c r="B43" s="75" t="s">
+      <c r="A43" s="74" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="76" t="s">
         <v>6</v>
       </c>
       <c r="C43" s="3">
@@ -4062,7 +4110,7 @@
       <c r="BE43" s="2"/>
     </row>
     <row r="44" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B44" s="76"/>
+      <c r="B44" s="77"/>
       <c r="C44">
         <v>0</v>
       </c>
@@ -4088,7 +4136,7 @@
       <c r="BE44" s="2"/>
     </row>
     <row r="45" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B45" s="76"/>
+      <c r="B45" s="77"/>
       <c r="C45">
         <v>0</v>
       </c>
@@ -4114,7 +4162,7 @@
       <c r="BE45" s="2"/>
     </row>
     <row r="46" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B46" s="76"/>
+      <c r="B46" s="77"/>
       <c r="C46">
         <v>0</v>
       </c>
@@ -4140,7 +4188,7 @@
       <c r="BE46" s="2"/>
     </row>
     <row r="47" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B47" s="76"/>
+      <c r="B47" s="77"/>
       <c r="C47">
         <v>0</v>
       </c>
@@ -4166,7 +4214,7 @@
       <c r="BE47" s="2"/>
     </row>
     <row r="48" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B48" s="76"/>
+      <c r="B48" s="77"/>
       <c r="C48">
         <v>0</v>
       </c>
@@ -4199,10 +4247,10 @@
       <c r="BE49" s="2"/>
     </row>
     <row r="50" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="96" t="s">
-        <v>96</v>
-      </c>
-      <c r="B50" s="97"/>
+      <c r="A50" s="93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B50" s="94"/>
       <c r="C50">
         <f t="array" ref="C50:H55">MMULT(C33:H38,C43:H48)</f>
         <v>0</v>
@@ -4229,8 +4277,8 @@
       <c r="BE50" s="2"/>
     </row>
     <row r="51" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A51" s="97"/>
-      <c r="B51" s="97"/>
+      <c r="A51" s="94"/>
+      <c r="B51" s="94"/>
       <c r="C51">
         <v>0</v>
       </c>
@@ -4256,8 +4304,8 @@
       <c r="BE51" s="2"/>
     </row>
     <row r="52" spans="1:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="97"/>
-      <c r="B52" s="97"/>
+      <c r="A52" s="94"/>
+      <c r="B52" s="94"/>
       <c r="C52">
         <v>0</v>
       </c>
@@ -4478,10 +4526,10 @@
       <c r="BE72" s="2"/>
     </row>
     <row r="73" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B73" s="80" t="s">
-        <v>75</v>
-      </c>
-      <c r="C73" s="76"/>
+      <c r="B73" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="C73" s="77"/>
       <c r="I73" s="2"/>
       <c r="AG73" s="4"/>
       <c r="AH73" s="4"/>
@@ -4489,10 +4537,10 @@
       <c r="BE73" s="2"/>
     </row>
     <row r="74" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B74" s="79" t="s">
+      <c r="B74" s="82" t="s">
         <v>32</v>
       </c>
-      <c r="C74" s="76"/>
+      <c r="C74" s="77"/>
       <c r="I74" s="2"/>
       <c r="AG74" s="4"/>
       <c r="AH74" s="4"/>
@@ -4504,7 +4552,7 @@
         <v>38</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I75" s="2"/>
       <c r="AG75" s="4"/>
@@ -4519,10 +4567,10 @@
       <c r="C76" s="67">
         <v>0.1</v>
       </c>
-      <c r="D76" s="78" t="s">
-        <v>77</v>
-      </c>
-      <c r="E76" s="76"/>
+      <c r="D76" s="86" t="s">
+        <v>76</v>
+      </c>
+      <c r="E76" s="77"/>
       <c r="I76" s="2"/>
       <c r="AG76" s="4"/>
       <c r="AH76" s="4"/>
@@ -4531,15 +4579,15 @@
     </row>
     <row r="77" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B77" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C77" s="68" t="s">
+        <v>77</v>
+      </c>
+      <c r="D77" s="86" t="s">
         <v>78</v>
       </c>
-      <c r="C77" s="68" t="s">
-        <v>78</v>
-      </c>
-      <c r="D77" s="78" t="s">
-        <v>79</v>
-      </c>
-      <c r="E77" s="76"/>
+      <c r="E77" s="77"/>
       <c r="I77" s="2"/>
       <c r="AG77" s="4"/>
       <c r="AH77" s="4"/>
@@ -4547,8 +4595,8 @@
       <c r="BE77" s="2"/>
     </row>
     <row r="78" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="D78" s="78"/>
-      <c r="E78" s="76"/>
+      <c r="D78" s="86"/>
+      <c r="E78" s="77"/>
       <c r="I78" s="2"/>
       <c r="AG78" s="4"/>
       <c r="AH78" s="4"/>
@@ -4556,12 +4604,12 @@
       <c r="BE78" s="2"/>
     </row>
     <row r="79" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B79" s="80" t="s">
-        <v>80</v>
-      </c>
-      <c r="C79" s="76"/>
-      <c r="D79" s="78"/>
-      <c r="E79" s="76"/>
+      <c r="B79" s="83" t="s">
+        <v>79</v>
+      </c>
+      <c r="C79" s="77"/>
+      <c r="D79" s="86"/>
+      <c r="E79" s="77"/>
       <c r="I79" s="2"/>
       <c r="AG79" s="4"/>
       <c r="AH79" s="4"/>
@@ -4569,12 +4617,12 @@
       <c r="BE79" s="2"/>
     </row>
     <row r="80" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="B80" s="79" t="s">
+      <c r="B80" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="C80" s="76"/>
-      <c r="D80" s="78"/>
-      <c r="E80" s="76"/>
+      <c r="C80" s="77"/>
+      <c r="D80" s="86"/>
+      <c r="E80" s="77"/>
       <c r="I80" s="2"/>
       <c r="AG80" s="4"/>
       <c r="AH80" s="4"/>
@@ -4583,13 +4631,13 @@
     </row>
     <row r="81" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B81" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C81" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="C81" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="D81" s="78"/>
-      <c r="E81" s="76"/>
+      <c r="D81" s="86"/>
+      <c r="E81" s="77"/>
       <c r="I81" s="2"/>
       <c r="AG81" s="4"/>
       <c r="AH81" s="4"/>
@@ -4603,10 +4651,10 @@
       <c r="C82" s="39">
         <v>3</v>
       </c>
-      <c r="D82" s="78" t="s">
-        <v>81</v>
-      </c>
-      <c r="E82" s="76"/>
+      <c r="D82" s="86" t="s">
+        <v>80</v>
+      </c>
+      <c r="E82" s="77"/>
       <c r="I82" s="2"/>
       <c r="AG82" s="4"/>
       <c r="AH82" s="4"/>
@@ -4615,15 +4663,15 @@
     </row>
     <row r="83" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B83" s="69" t="s">
+        <v>81</v>
+      </c>
+      <c r="C83" s="69" t="s">
         <v>82</v>
       </c>
-      <c r="C83" s="69" t="s">
+      <c r="D83" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="D83" s="78" t="s">
-        <v>84</v>
-      </c>
-      <c r="E83" s="76"/>
+      <c r="E83" s="77"/>
       <c r="I83" s="2"/>
       <c r="AG83" s="4"/>
       <c r="AH83" s="4"/>
@@ -4646,7 +4694,7 @@
     </row>
     <row r="86" spans="2:57" ht="12.75" x14ac:dyDescent="0.2">
       <c r="B86" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="I86" s="2"/>
       <c r="AG86" s="4"/>
@@ -11061,6 +11109,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="AL4:AO4"/>
+    <mergeCell ref="B43:B48"/>
+    <mergeCell ref="C42:H42"/>
+    <mergeCell ref="AJ14:AO14"/>
+    <mergeCell ref="D79:E79"/>
+    <mergeCell ref="B74:C74"/>
+    <mergeCell ref="B73:C73"/>
+    <mergeCell ref="B10:B15"/>
+    <mergeCell ref="D80:E80"/>
+    <mergeCell ref="D82:E82"/>
+    <mergeCell ref="D81:E81"/>
+    <mergeCell ref="D83:E83"/>
+    <mergeCell ref="AC4:AD4"/>
+    <mergeCell ref="T4:Y4"/>
+    <mergeCell ref="E19:H19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C18:H18"/>
+    <mergeCell ref="K5:K9"/>
+    <mergeCell ref="K15:K19"/>
+    <mergeCell ref="F10:G15"/>
+    <mergeCell ref="Z2:AB2"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="B79:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="A50:B52"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B23:B26"/>
+    <mergeCell ref="A21:A26"/>
+    <mergeCell ref="B33:B34"/>
+    <mergeCell ref="A30:B32"/>
+    <mergeCell ref="D77:E77"/>
+    <mergeCell ref="D78:E78"/>
+    <mergeCell ref="B35:B38"/>
+    <mergeCell ref="E31:H31"/>
+    <mergeCell ref="D76:E76"/>
     <mergeCell ref="A33:A38"/>
     <mergeCell ref="BF1:BK3"/>
     <mergeCell ref="BG5:BI6"/>
@@ -11077,42 +11161,6 @@
     <mergeCell ref="C12:C15"/>
     <mergeCell ref="M14:R14"/>
     <mergeCell ref="C10:C11"/>
-    <mergeCell ref="Z2:AB2"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="B79:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="A50:B52"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B26"/>
-    <mergeCell ref="A21:A26"/>
-    <mergeCell ref="B33:B34"/>
-    <mergeCell ref="A30:B32"/>
-    <mergeCell ref="D77:E77"/>
-    <mergeCell ref="D78:E78"/>
-    <mergeCell ref="B35:B38"/>
-    <mergeCell ref="E31:H31"/>
-    <mergeCell ref="D76:E76"/>
-    <mergeCell ref="D80:E80"/>
-    <mergeCell ref="D82:E82"/>
-    <mergeCell ref="D81:E81"/>
-    <mergeCell ref="D83:E83"/>
-    <mergeCell ref="AC4:AD4"/>
-    <mergeCell ref="T4:Y4"/>
-    <mergeCell ref="E19:H19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C18:H18"/>
-    <mergeCell ref="K5:K9"/>
-    <mergeCell ref="K15:K19"/>
-    <mergeCell ref="F10:G15"/>
-    <mergeCell ref="AL4:AO4"/>
-    <mergeCell ref="B43:B48"/>
-    <mergeCell ref="C42:H42"/>
-    <mergeCell ref="AJ14:AO14"/>
-    <mergeCell ref="D79:E79"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B73:C73"/>
-    <mergeCell ref="B10:B15"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>